<commit_message>
Update Bulk User Upload Template with new data structure
</commit_message>
<xml_diff>
--- a/public/BulkUserUploadTemplate.xlsx
+++ b/public/BulkUserUploadTemplate.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZEMU\9.MINE\zemu\Files\My Training Areas\INSA\Personality test frontend\INSA-PersonalityTest-saas-web-app\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671079B3-F898-42EC-A786-B02DABEBC8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2184" windowWidth="17280" windowHeight="8880" xr2:uid="{27586D78-9F7B-4A4B-9220-B4C81AB4BD2F}"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,12 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+  <si>
+    <t>Full Name</t>
   </si>
   <si>
     <t>Email Address</t>
@@ -54,29 +42,301 @@
   </si>
   <si>
     <t>Department</t>
+  </si>
+  <si>
+    <t>Aklilu Haile Abitew</t>
+  </si>
+  <si>
+    <t>akilshm9631@gmail.com</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>there</t>
+  </si>
+  <si>
+    <t>Asregdew Mesele Shibeshi</t>
+  </si>
+  <si>
+    <t>asregedewm@gmail.com</t>
+  </si>
+  <si>
+    <t>Balcha Debebe Tadesse</t>
+  </si>
+  <si>
+    <t>balcha.ta@gmail.com</t>
+  </si>
+  <si>
+    <t>Bezialem Sintayehu Gebru</t>
+  </si>
+  <si>
+    <t>bezihalem24@gmail.com</t>
+  </si>
+  <si>
+    <t>Biniyam Mersha Haile</t>
+  </si>
+  <si>
+    <t>biniammer@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Walellgn </t>
+  </si>
+  <si>
+    <t>walellgndaniel@gmail.com</t>
+  </si>
+  <si>
+    <t>Endale Shiferaw Worku</t>
+  </si>
+  <si>
+    <t>endaleshiferaw270@gmail.com</t>
+  </si>
+  <si>
+    <t>Girum Zena Tegegn</t>
+  </si>
+  <si>
+    <t>girumzena@gmail.com</t>
+  </si>
+  <si>
+    <t>Merid Kebede Weldeyes</t>
+  </si>
+  <si>
+    <t>kebedemerid212@gmail.com</t>
+  </si>
+  <si>
+    <t>Muche Ambisa Yadesa</t>
+  </si>
+  <si>
+    <t>mucheastu7@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigussie Kebede </t>
+  </si>
+  <si>
+    <t>negussiekebede06@gmail.com</t>
+  </si>
+  <si>
+    <t>Sori Milkesa Gonfa</t>
+  </si>
+  <si>
+    <t>milkesasor877@gmail.com</t>
+  </si>
+  <si>
+    <t>Tesfaye Borcha Bololo</t>
+  </si>
+  <si>
+    <t>tesfayeboricha7@gmail.com</t>
+  </si>
+  <si>
+    <t>Yoseph Birhanu Tassew</t>
+  </si>
+  <si>
+    <t>yosephrich123@gmail.com</t>
+  </si>
+  <si>
+    <t>Sileshi Demisse Borena</t>
+  </si>
+  <si>
+    <t>sileshidemissie.41@gmail.com</t>
+  </si>
+  <si>
+    <t>Bereket Bogale</t>
+  </si>
+  <si>
+    <t>bekayaeng@gmail.com</t>
+  </si>
+  <si>
+    <t>Sr. Telelech Befikadu</t>
+  </si>
+  <si>
+    <t>teleb@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,10 +346,197 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -97,27 +544,331 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="25"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -166,7 +917,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -199,26 +950,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -251,23 +985,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -429,34 +1146,28 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD64651-92EA-4F74-8DA9-A244B1A95383}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="A2:F6"/>
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="22.4444444444444" customWidth="1"/>
+    <col min="3" max="3" width="14.1111111111111" customWidth="1"/>
+    <col min="4" max="4" width="9.66666666666667" customWidth="1"/>
+    <col min="5" max="5" width="11.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,12 +1183,318 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" ht="15.6" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>2519478597</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="15.6" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2519478598</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="15.6" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>2519478599</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" ht="15.6" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>2519478600</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" ht="15.6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>2519478601</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" ht="15.6" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>2519478602</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" ht="15.6" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>2519478603</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" ht="15.6" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>2519478604</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" ht="15.6" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>2519478605</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" ht="15.6" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>2519478606</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" ht="15.6" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>2519478607</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" ht="15.6" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>2519478608</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" ht="15.6" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>2519478609</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" ht="15.6" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>2519478610</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" ht="15.6" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>2519478611</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" ht="15.6" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>2519478612</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" ht="15.6" spans="1:5">
+      <c r="A18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>2519478613</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="biniammer@gmail.com"/>
+    <hyperlink ref="B17" r:id="rId2" display="bekayaeng@gmail.com"/>
+    <hyperlink ref="B12" r:id="rId3" display="negussiekebede06@gmail.com"/>
+    <hyperlink ref="B15" r:id="rId4" display="yosephrich123@gmail.com"/>
+    <hyperlink ref="B13" r:id="rId5" display="milkesasor877@gmail.com"/>
+    <hyperlink ref="B14" r:id="rId6" display="tesfayeboricha7@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId7" display="kebedemerid212@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId8" display="asregedewm@gmail.com"/>
+    <hyperlink ref="B11" r:id="rId9" display="mucheastu7@gmail.com"/>
+    <hyperlink ref="B16" r:id="rId10" display="sileshidemissie.41@gmail.com"/>
+    <hyperlink ref="B7" r:id="rId11" display="walellgndaniel@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId12" display="bezihalem24@gmail.com"/>
+    <hyperlink ref="B9" r:id="rId13" display="girumzena@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId14" display="akilshm9631@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId15" display="balcha.ta@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId16" display="endaleshiferaw270@gmail.com"/>
+    <hyperlink ref="B18" r:id="rId17" display="teleb@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>